<commit_message>
publish pins bug fixed
</commit_message>
<xml_diff>
--- a/docs/Kupongo UAT.xlsx
+++ b/docs/Kupongo UAT.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="78">
   <si>
     <t>TC #</t>
   </si>
@@ -167,9 +167,6 @@
     <t xml:space="preserve">Email, Password </t>
   </si>
   <si>
-    <t>first name, last name, Email</t>
-  </si>
-  <si>
     <t xml:space="preserve">None </t>
   </si>
   <si>
@@ -209,13 +206,61 @@
     <t>An invalid Collection Start Date is after the Collect End Date, an invalid Collection End Date is before the Collection Start Date, an invalid  Redemption Start Date is  before the Collection Start Date, an invalid Redemption End Date is before the Redemption Start Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Create Template verify  unique QR Image generated </t>
-  </si>
-  <si>
     <t xml:space="preserve">Publish Pins verify default dates set </t>
   </si>
   <si>
     <t>Default dates: preViewingDate defaults to date of pinning, collectStartDate defaults to date of pinning, collectEndDate defaults to collectStartDate + 24 hrs,  redeemStartDate defaults to date of pinning, redeemEndDate defaults to date of pinning + 30 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Template verify unique QR Image generated </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter valid Company Name and User Token and press the Register button </t>
+  </si>
+  <si>
+    <t>Enter an invalid Company Name or User Token and press the Register button</t>
+  </si>
+  <si>
+    <t>Enter invalid Email or Password and press the Login button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter valid Email and Password and press the Login button </t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Enter valid email, press reset button, and check email</t>
+  </si>
+  <si>
+    <t>Enter, at a minimum,  a Title and a valid UPC Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">press cancel buttom on Template Creation window </t>
+  </si>
+  <si>
+    <t>Enter invalid UPC Code, attempt to save without Title or UPC Code</t>
+  </si>
+  <si>
+    <t>press delete button on Template Thumbnail and delete button on confirmation popup</t>
+  </si>
+  <si>
+    <t>press delete button on Template Thumbnail cancel button on confirmation popup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select Template Thumbnail and click within the area of the map </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single click on Pin Marker and press the delete button on the popup </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter at a minimum a valid Title, Collection Start Date, Collection End Date, Redemption Start Date, and Redemption End Date </t>
+  </si>
+  <si>
+    <t xml:space="preserve">press cancel button on Publish Pins window </t>
+  </si>
+  <si>
+    <t xml:space="preserve">press cancel button on Template Edit window </t>
   </si>
 </sst>
 </file>
@@ -571,18 +616,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="48" customWidth="1"/>
     <col min="5" max="5" width="35" customWidth="1"/>
-    <col min="6" max="6" width="30.83203125" customWidth="1"/>
+    <col min="6" max="6" width="30.1640625" customWidth="1"/>
     <col min="7" max="7" width="21.33203125" customWidth="1"/>
     <col min="8" max="8" width="32.1640625" customWidth="1"/>
-    <col min="9" max="9" width="22.6640625" customWidth="1"/>
+    <col min="9" max="9" width="41.1640625" customWidth="1"/>
     <col min="10" max="10" width="22.1640625" customWidth="1"/>
     <col min="11" max="11" width="21.33203125" customWidth="1"/>
     <col min="12" max="12" width="21.6640625" customWidth="1"/>
@@ -626,7 +669,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -645,7 +688,9 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
@@ -669,14 +714,16 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I3" s="4"/>
+        <v>56</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -695,7 +742,9 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="I4" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
@@ -719,14 +768,16 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I5" s="4"/>
+        <v>51</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -740,17 +791,19 @@
         <v>22</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="I6" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -764,17 +817,19 @@
         <v>28</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="I7" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -788,17 +843,19 @@
         <v>30</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="I8" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -812,19 +869,21 @@
         <v>24</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="4"/>
+        <v>57</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -838,12 +897,14 @@
         <v>22</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="I10" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
@@ -862,17 +923,19 @@
         <v>22</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="I11" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -886,17 +949,19 @@
         <v>23</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="I12" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -910,17 +975,19 @@
         <v>30</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="I13" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -934,17 +1001,19 @@
         <v>30</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="I14" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -958,19 +1027,21 @@
         <v>22</v>
       </c>
       <c r="E15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="I15" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -984,14 +1055,16 @@
         <v>22</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="I16" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
@@ -1010,12 +1083,14 @@
         <v>22</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="I17" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
@@ -1034,12 +1109,14 @@
         <v>22</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="I18" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
@@ -1058,12 +1135,12 @@
         <v>23</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
@@ -1084,7 +1161,7 @@
         <v>22</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -1108,7 +1185,7 @@
         <v>22</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -1132,7 +1209,7 @@
         <v>23</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -1156,7 +1233,7 @@
         <v>22</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -1180,7 +1257,7 @@
         <v>22</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -1195,7 +1272,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>18</v>
@@ -1204,7 +1281,7 @@
         <v>22</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -1219,7 +1296,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>18</v>
@@ -1228,12 +1305,12 @@
         <v>30</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>

</xml_diff>